<commit_message>
Version de l'outil d'importation incluant les 10 fruits et légumes.
</commit_message>
<xml_diff>
--- a/OutilImportation/OutilImportation/infoleg.xlsx
+++ b/OutilImportation/OutilImportation/infoleg.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Franc\Documents\Cegep\Projet\GreenHouse-Tech\OutilImportation\OutilImportation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5A46013-27E7-4003-8021-F49A057C94A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41176A6B-D847-4E7B-A0E0-7F5B593D0664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4815" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="59">
   <si>
     <t>Voisinage favorable</t>
   </si>
@@ -33,9 +33,6 @@
     <t>Concombre</t>
   </si>
   <si>
-    <t>Semez en poquets* de 5 graines. Gardez 3 plants par poquet*.</t>
-  </si>
-  <si>
     <t>Tomate</t>
   </si>
   <si>
@@ -105,9 +102,6 @@
     <t>Nb jours de maturation</t>
   </si>
   <si>
-    <t>Cm entre plant max</t>
-  </si>
-  <si>
     <t>Cm entre plant min</t>
   </si>
   <si>
@@ -120,13 +114,94 @@
     <t>Humidité min (%)</t>
   </si>
   <si>
-    <t>Température max (°C)</t>
-  </si>
-  <si>
     <t>Température min (°C)</t>
   </si>
   <si>
     <t>Nom aliment</t>
+  </si>
+  <si>
+    <t>Cm entre plant rang min</t>
+  </si>
+  <si>
+    <t>PH min</t>
+  </si>
+  <si>
+    <t>PH max</t>
+  </si>
+  <si>
+    <t>Semez en poquets de 5 graines. Gardez 3 plants par poquet.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> les courgettes poussent  sur la plupart des sols.</t>
+  </si>
+  <si>
+    <t>Carotte</t>
+  </si>
+  <si>
+    <t>Chou, haricot, laitue, oignon, piment, poireau, pois, radis, salsifis, tomate</t>
+  </si>
+  <si>
+    <t>Semez aux 15 jours du début mai au 15 juin.</t>
+  </si>
+  <si>
+    <t>meuble, riche, dépourvu de cailloux</t>
+  </si>
+  <si>
+    <t>Melon</t>
+  </si>
+  <si>
+    <t>Maïs</t>
+  </si>
+  <si>
+    <t>Semez en poquets de 3 graines. Gardez 3 ou 4 fruits par plant. Le melon n’aime pas les courants d’air.</t>
+  </si>
+  <si>
+    <t>profond, bien drainé, riche en matières organiques</t>
+  </si>
+  <si>
+    <t>Betterave, concombre, citrouille, haricot, melon, pois, pomme de terre</t>
+  </si>
+  <si>
+    <t>Semez sur au moins deux rangs pour favoriser la pollinisation.</t>
+  </si>
+  <si>
+    <t>profond, léger, frais et riche en humus,</t>
+  </si>
+  <si>
+    <t>Épinard</t>
+  </si>
+  <si>
+    <t>Chou, laitue, poireau, radis</t>
+  </si>
+  <si>
+    <t>Semez tôt au printemps ou à la fin de l'été, sinon risque de monter en graines.</t>
+  </si>
+  <si>
+    <t>Meuble, frais et humifère</t>
+  </si>
+  <si>
+    <t>Citrouille</t>
+  </si>
+  <si>
+    <t>Laitue, maïs, pois, radis</t>
+  </si>
+  <si>
+    <t>Semez en poquets de 3 graines. Gardez 2 à 4 fruits par plant.</t>
+  </si>
+  <si>
+    <t>loam sableux,sol bien drainé et les sols argileux</t>
+  </si>
+  <si>
+    <t>Framboise</t>
+  </si>
+  <si>
+    <t>il accepte tous les voisinages et est accepté par tous</t>
+  </si>
+  <si>
+    <t>Les framboisiers s'accommodent de la mi-ombre, mais ils produisent des fruits plus sucrés et en plus grand nombre s'ils sont plantés au soleil.</t>
+  </si>
+  <si>
+    <t>humide, meuble, bien drainé, légèrement acide et fertile</t>
   </si>
 </sst>
 </file>
@@ -142,8 +217,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -151,15 +227,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -174,14 +249,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFDDEBF7"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -209,49 +284,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -529,10 +581,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -545,222 +597,554 @@
     <col min="6" max="6" width="24.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:16" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="1">
+        <v>30</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="9" t="s">
+    </row>
+    <row r="2" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>20</v>
+      </c>
+      <c r="C2" s="3">
+        <v>30</v>
+      </c>
+      <c r="D2" s="3">
+        <v>60</v>
+      </c>
+      <c r="E2" s="3">
+        <v>70</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="3">
+        <v>120</v>
+      </c>
+      <c r="H2" s="3">
+        <v>120</v>
+      </c>
+      <c r="I2" s="3">
+        <v>60</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" s="4">
+        <v>7</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O2" s="3">
+        <v>6</v>
+      </c>
+      <c r="P2" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="3">
+        <v>25</v>
+      </c>
+      <c r="C3" s="3">
+        <v>30</v>
+      </c>
+      <c r="D3" s="3">
+        <v>65</v>
+      </c>
+      <c r="E3" s="3">
+        <v>80</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="3">
+        <v>80</v>
+      </c>
+      <c r="H3" s="3">
+        <v>80</v>
+      </c>
+      <c r="I3" s="3">
+        <v>60</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M3" s="4">
+        <v>10</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O3" s="3">
+        <v>5.6</v>
+      </c>
+      <c r="P3" s="3">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="3">
+        <v>18</v>
+      </c>
+      <c r="C4" s="3">
+        <v>22</v>
+      </c>
+      <c r="D4" s="3">
+        <v>70</v>
+      </c>
+      <c r="E4" s="3">
+        <v>80</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="3">
+        <v>40</v>
+      </c>
+      <c r="H4" s="3">
+        <v>50</v>
+      </c>
+      <c r="I4" s="3">
+        <v>40</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M4" s="4">
+        <v>7</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="O4" s="3">
+        <v>5.8</v>
+      </c>
+      <c r="P4" s="3">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="3">
+        <v>18</v>
+      </c>
+      <c r="C5" s="3">
+        <v>22</v>
+      </c>
+      <c r="D5" s="3">
+        <v>75</v>
+      </c>
+      <c r="E5" s="3">
+        <v>75</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="3">
+        <v>45</v>
+      </c>
+      <c r="H5" s="3">
+        <v>90</v>
+      </c>
+      <c r="I5" s="3">
+        <v>70</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="M5" s="4">
+        <v>5</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="O5" s="3">
+        <v>6</v>
+      </c>
+      <c r="P5" s="3">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="3">
+        <v>8</v>
+      </c>
+      <c r="C6" s="3">
+        <v>29</v>
+      </c>
+      <c r="D6" s="3">
+        <v>70</v>
+      </c>
+      <c r="E6" s="3">
+        <v>75</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="3">
+        <v>5</v>
+      </c>
+      <c r="H6" s="3">
+        <v>45</v>
+      </c>
+      <c r="I6" s="3">
+        <v>60</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="M6" s="3">
+        <v>90</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O6" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="P6" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="144" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="3">
+        <v>12</v>
+      </c>
+      <c r="C7" s="3">
+        <v>20</v>
+      </c>
+      <c r="D7" s="3">
+        <v>85</v>
+      </c>
+      <c r="E7" s="3">
+        <v>90</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="3">
+        <v>150</v>
+      </c>
+      <c r="H7" s="3">
+        <v>200</v>
+      </c>
+      <c r="I7" s="3">
+        <v>80</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="M7" s="3">
+        <v>21</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O7" s="3">
+        <v>7</v>
+      </c>
+      <c r="P7" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="3">
+        <v>25</v>
+      </c>
+      <c r="C8" s="3">
+        <v>33</v>
+      </c>
+      <c r="D8" s="3">
+        <v>70</v>
+      </c>
+      <c r="E8" s="3">
+        <v>80</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="3">
+        <v>25</v>
+      </c>
+      <c r="H8" s="3">
+        <v>75</v>
+      </c>
+      <c r="I8" s="3">
+        <v>70</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="M8" s="3">
+        <v>90</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O8" s="3">
+        <v>6</v>
+      </c>
+      <c r="P8" s="3">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="3">
+        <v>7</v>
+      </c>
+      <c r="C9" s="3">
+        <v>24</v>
+      </c>
+      <c r="D9" s="3">
+        <v>70</v>
+      </c>
+      <c r="E9" s="3">
+        <v>80</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" s="3">
+        <v>10</v>
+      </c>
+      <c r="H9" s="3">
+        <v>40</v>
+      </c>
+      <c r="I9" s="3">
+        <v>50</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="M9" s="3">
+        <v>14</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O9" s="3">
+        <v>6.5</v>
+      </c>
+      <c r="P9" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="3">
+        <v>21</v>
+      </c>
+      <c r="C10" s="3">
         <v>32</v>
       </c>
-      <c r="C1" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" s="9" t="s">
+      <c r="D10" s="3">
+        <v>50</v>
+      </c>
+      <c r="E10" s="3">
+        <v>70</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G10" s="3">
+        <v>200</v>
+      </c>
+      <c r="H10" s="3">
+        <v>250</v>
+      </c>
+      <c r="I10" s="3">
+        <v>120</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="M10" s="3">
+        <v>180</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O10" s="3">
+        <v>6.5</v>
+      </c>
+      <c r="P10" s="3">
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" s="3">
+        <v>20</v>
+      </c>
+      <c r="C11" s="3">
         <v>30</v>
       </c>
-      <c r="E1" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="L1" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="N1" s="9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>20</v>
-      </c>
-      <c r="C2" s="1">
-        <v>30</v>
-      </c>
-      <c r="D2" s="1">
-        <v>60</v>
-      </c>
-      <c r="E2" s="1">
+      <c r="D11" s="3">
         <v>70</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="1">
+      <c r="E11" s="3">
+        <v>80</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="3">
+        <v>45</v>
+      </c>
+      <c r="H11" s="3">
         <v>120</v>
       </c>
-      <c r="H2" s="1">
-        <v>120</v>
-      </c>
-      <c r="I2" s="1">
-        <v>60</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" s="7" t="s">
+      <c r="I11" s="3">
+        <v>50</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="M11" s="3">
         <v>2</v>
       </c>
-      <c r="L2" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="M2" s="2">
-        <v>7</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="1">
-        <v>25</v>
-      </c>
-      <c r="C3" s="1">
-        <v>30</v>
-      </c>
-      <c r="D3" s="1">
-        <v>65</v>
-      </c>
-      <c r="E3" s="1">
-        <v>80</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="1">
-        <v>80</v>
-      </c>
-      <c r="H3" s="1">
-        <v>80</v>
-      </c>
-      <c r="I3" s="1">
-        <v>60</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="K3" s="7"/>
-      <c r="L3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="M3" s="2">
-        <v>10</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="1">
-        <v>18</v>
-      </c>
-      <c r="C4" s="1">
-        <v>22</v>
-      </c>
-      <c r="D4" s="1">
-        <v>70</v>
-      </c>
-      <c r="E4" s="1">
-        <v>80</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="1">
-        <v>40</v>
-      </c>
-      <c r="H4" s="1">
-        <v>50</v>
-      </c>
-      <c r="I4" s="1">
-        <v>40</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K4" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="M4" s="2">
-        <v>7</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1">
-        <v>18</v>
-      </c>
-      <c r="C5" s="1">
-        <v>22</v>
-      </c>
-      <c r="D5" s="4">
-        <v>75</v>
-      </c>
-      <c r="E5" s="1">
-        <v>75</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" s="1">
-        <v>45</v>
-      </c>
-      <c r="H5" s="1">
-        <v>90</v>
-      </c>
-      <c r="I5" s="1">
-        <v>70</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="K5" s="3" t="s">
+      <c r="N11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="L5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="M5" s="2">
-        <v>5</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>5</v>
+      <c r="O11" s="3">
+        <v>5.8</v>
+      </c>
+      <c r="P11" s="3">
+        <v>6.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modification plantType dans l'outil d'importation.
</commit_message>
<xml_diff>
--- a/OutilImportation/OutilImportation/infoleg.xlsx
+++ b/OutilImportation/OutilImportation/infoleg.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Franc\Documents\Cegep\Projet\GreenHouse-Tech\OutilImportation\OutilImportation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41176A6B-D847-4E7B-A0E0-7F5B593D0664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A308A645-D3AB-4514-9752-71E8851170B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -66,9 +66,6 @@
     <t>Fraise</t>
   </si>
   <si>
-    <t>Légume</t>
-  </si>
-  <si>
     <t>Matière organique fraîche</t>
   </si>
   <si>
@@ -202,6 +199,9 @@
   </si>
   <si>
     <t>humide, meuble, bien drainé, légèrement acide et fertile</t>
+  </si>
+  <si>
+    <t>Vegetable</t>
   </si>
 </sst>
 </file>
@@ -583,8 +583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -599,52 +599,52 @@
   <sheetData>
     <row r="1" spans="1:16" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C1" s="1">
         <v>30</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -664,7 +664,7 @@
         <v>70</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G2" s="3">
         <v>120</v>
@@ -676,19 +676,19 @@
         <v>60</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M2" s="4">
         <v>7</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>13</v>
+        <v>58</v>
       </c>
       <c r="O2" s="3">
         <v>6</v>
@@ -699,7 +699,7 @@
     </row>
     <row r="3" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="3">
         <v>25</v>
@@ -714,7 +714,7 @@
         <v>80</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G3" s="3">
         <v>80</v>
@@ -726,19 +726,19 @@
         <v>60</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M3" s="4">
         <v>10</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>13</v>
+        <v>58</v>
       </c>
       <c r="O3" s="3">
         <v>5.6</v>
@@ -849,7 +849,7 @@
     </row>
     <row r="6" spans="1:16" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B6" s="3">
         <v>8</v>
@@ -876,19 +876,19 @@
         <v>60</v>
       </c>
       <c r="J6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="K6" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="L6" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>39</v>
       </c>
       <c r="M6" s="3">
         <v>90</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>13</v>
+        <v>58</v>
       </c>
       <c r="O6" s="3">
         <v>5.5</v>
@@ -899,7 +899,7 @@
     </row>
     <row r="7" spans="1:16" ht="144" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B7" s="3">
         <v>12</v>
@@ -926,19 +926,19 @@
         <v>80</v>
       </c>
       <c r="J7" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="K7" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="K7" s="3" t="s">
+      <c r="L7" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>43</v>
       </c>
       <c r="M7" s="3">
         <v>21</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>13</v>
+        <v>58</v>
       </c>
       <c r="O7" s="3">
         <v>7</v>
@@ -949,7 +949,7 @@
     </row>
     <row r="8" spans="1:16" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B8" s="3">
         <v>25</v>
@@ -976,19 +976,19 @@
         <v>70</v>
       </c>
       <c r="J8" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="K8" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="K8" s="3" t="s">
+      <c r="L8" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="L8" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="M8" s="3">
         <v>90</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>13</v>
+        <v>58</v>
       </c>
       <c r="O8" s="3">
         <v>6</v>
@@ -999,7 +999,7 @@
     </row>
     <row r="9" spans="1:16" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B9" s="3">
         <v>7</v>
@@ -1026,19 +1026,19 @@
         <v>50</v>
       </c>
       <c r="J9" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="K9" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="K9" s="3" t="s">
+      <c r="L9" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>50</v>
       </c>
       <c r="M9" s="3">
         <v>14</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>13</v>
+        <v>58</v>
       </c>
       <c r="O9" s="3">
         <v>6.5</v>
@@ -1049,7 +1049,7 @@
     </row>
     <row r="10" spans="1:16" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B10" s="3">
         <v>21</v>
@@ -1076,19 +1076,19 @@
         <v>120</v>
       </c>
       <c r="J10" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K10" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="K10" s="3" t="s">
+      <c r="L10" s="3" t="s">
         <v>53</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>54</v>
       </c>
       <c r="M10" s="3">
         <v>180</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>13</v>
+        <v>58</v>
       </c>
       <c r="O10" s="3">
         <v>6.5</v>
@@ -1099,7 +1099,7 @@
     </row>
     <row r="11" spans="1:16" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B11" s="3">
         <v>20</v>
@@ -1126,13 +1126,13 @@
         <v>50</v>
       </c>
       <c r="J11" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="K11" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="K11" s="3" t="s">
+      <c r="L11" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="L11" s="3" t="s">
-        <v>58</v>
       </c>
       <c r="M11" s="3">
         <v>2</v>
@@ -1160,15 +1160,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F8E4E3B306EF3243B17A3CCFA9E9441A" ma:contentTypeVersion="5" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="6b288f72ed777e9b1aae4ed183f5678c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7a2aa5ce-9268-4b11-b8eb-4b0ce9691849" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fb49ff9540079cd935bf7e769512398a" ns2:_="">
     <xsd:import namespace="7a2aa5ce-9268-4b11-b8eb-4b0ce9691849"/>
@@ -1318,6 +1309,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5A09CFD-DE79-4514-8D9E-8327453187AE}">
   <ds:schemaRefs>
@@ -1328,14 +1328,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F9B1BA4-1007-4EDD-9D02-AF3339A6D0CD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73027F6-8459-4821-9782-8EA37E764BC2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1351,4 +1343,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F9B1BA4-1007-4EDD-9D02-AF3339A6D0CD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Request #035 Barre de recherches terminée.
</commit_message>
<xml_diff>
--- a/OutilImportation/OutilImportation/infoleg.xlsx
+++ b/OutilImportation/OutilImportation/infoleg.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Franc\Documents\Cegep\Projet\GreenHouse-Tech\OutilImportation\OutilImportation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A308A645-D3AB-4514-9752-71E8851170B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B25A912-B50F-424D-9820-212748B751BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -583,7 +583,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
@@ -595,6 +595,7 @@
     <col min="4" max="4" width="19.6640625" customWidth="1"/>
     <col min="5" max="5" width="22.109375" customWidth="1"/>
     <col min="6" max="6" width="24.88671875" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="48" customHeight="1" x14ac:dyDescent="0.3">
@@ -1160,6 +1161,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F8E4E3B306EF3243B17A3CCFA9E9441A" ma:contentTypeVersion="5" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="6b288f72ed777e9b1aae4ed183f5678c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7a2aa5ce-9268-4b11-b8eb-4b0ce9691849" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fb49ff9540079cd935bf7e769512398a" ns2:_="">
     <xsd:import namespace="7a2aa5ce-9268-4b11-b8eb-4b0ce9691849"/>
@@ -1309,15 +1319,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5A09CFD-DE79-4514-8D9E-8327453187AE}">
   <ds:schemaRefs>
@@ -1328,6 +1329,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F9B1BA4-1007-4EDD-9D02-AF3339A6D0CD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73027F6-8459-4821-9782-8EA37E764BC2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1343,12 +1352,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F9B1BA4-1007-4EDD-9D02-AF3339A6D0CD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Modification nécessaires de l'API pour l'outil d'importation fait.  Outil d'importation utilise maintenant l'API.
</commit_message>
<xml_diff>
--- a/OutilImportation/OutilImportation/infoleg.xlsx
+++ b/OutilImportation/OutilImportation/infoleg.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Franc\Documents\Cegep\Projet\GreenHouse-Tech\OutilImportation\OutilImportation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B25A912-B50F-424D-9820-212748B751BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5881A83-A18F-4BA1-B3AF-4DBC44AFCD26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -165,43 +165,43 @@
     <t>profond, léger, frais et riche en humus,</t>
   </si>
   <si>
+    <t>Chou, laitue, poireau, radis</t>
+  </si>
+  <si>
+    <t>Semez tôt au printemps ou à la fin de l'été, sinon risque de monter en graines.</t>
+  </si>
+  <si>
+    <t>Meuble, frais et humifère</t>
+  </si>
+  <si>
+    <t>Citrouille</t>
+  </si>
+  <si>
+    <t>Laitue, maïs, pois, radis</t>
+  </si>
+  <si>
+    <t>Semez en poquets de 3 graines. Gardez 2 à 4 fruits par plant.</t>
+  </si>
+  <si>
+    <t>loam sableux,sol bien drainé et les sols argileux</t>
+  </si>
+  <si>
+    <t>Framboise</t>
+  </si>
+  <si>
+    <t>il accepte tous les voisinages et est accepté par tous</t>
+  </si>
+  <si>
+    <t>Les framboisiers s'accommodent de la mi-ombre, mais ils produisent des fruits plus sucrés et en plus grand nombre s'ils sont plantés au soleil.</t>
+  </si>
+  <si>
+    <t>humide, meuble, bien drainé, légèrement acide et fertile</t>
+  </si>
+  <si>
+    <t>Vegetable</t>
+  </si>
+  <si>
     <t>Épinard</t>
-  </si>
-  <si>
-    <t>Chou, laitue, poireau, radis</t>
-  </si>
-  <si>
-    <t>Semez tôt au printemps ou à la fin de l'été, sinon risque de monter en graines.</t>
-  </si>
-  <si>
-    <t>Meuble, frais et humifère</t>
-  </si>
-  <si>
-    <t>Citrouille</t>
-  </si>
-  <si>
-    <t>Laitue, maïs, pois, radis</t>
-  </si>
-  <si>
-    <t>Semez en poquets de 3 graines. Gardez 2 à 4 fruits par plant.</t>
-  </si>
-  <si>
-    <t>loam sableux,sol bien drainé et les sols argileux</t>
-  </si>
-  <si>
-    <t>Framboise</t>
-  </si>
-  <si>
-    <t>il accepte tous les voisinages et est accepté par tous</t>
-  </si>
-  <si>
-    <t>Les framboisiers s'accommodent de la mi-ombre, mais ils produisent des fruits plus sucrés et en plus grand nombre s'ils sont plantés au soleil.</t>
-  </si>
-  <si>
-    <t>humide, meuble, bien drainé, légèrement acide et fertile</t>
-  </si>
-  <si>
-    <t>Vegetable</t>
   </si>
 </sst>
 </file>
@@ -583,8 +583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -689,7 +689,7 @@
         <v>7</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O2" s="3">
         <v>6</v>
@@ -739,7 +739,7 @@
         <v>10</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O3" s="3">
         <v>5.6</v>
@@ -889,7 +889,7 @@
         <v>90</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O6" s="3">
         <v>5.5</v>
@@ -898,7 +898,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="144" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>39</v>
       </c>
@@ -939,7 +939,7 @@
         <v>21</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O7" s="3">
         <v>7</v>
@@ -989,7 +989,7 @@
         <v>90</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O8" s="3">
         <v>6</v>
@@ -998,9 +998,9 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="B9" s="3">
         <v>7</v>
@@ -1027,19 +1027,19 @@
         <v>50</v>
       </c>
       <c r="J9" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="K9" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="K9" s="3" t="s">
+      <c r="L9" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>49</v>
       </c>
       <c r="M9" s="3">
         <v>14</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O9" s="3">
         <v>6.5</v>
@@ -1050,7 +1050,7 @@
     </row>
     <row r="10" spans="1:16" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B10" s="3">
         <v>21</v>
@@ -1077,19 +1077,19 @@
         <v>120</v>
       </c>
       <c r="J10" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="K10" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="K10" s="3" t="s">
+      <c r="L10" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>53</v>
       </c>
       <c r="M10" s="3">
         <v>180</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O10" s="3">
         <v>6.5</v>
@@ -1098,9 +1098,9 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B11" s="3">
         <v>20</v>
@@ -1127,13 +1127,13 @@
         <v>50</v>
       </c>
       <c r="J11" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="K11" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="K11" s="3" t="s">
+      <c r="L11" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="L11" s="3" t="s">
-        <v>57</v>
       </c>
       <c r="M11" s="3">
         <v>2</v>
@@ -1161,15 +1161,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F8E4E3B306EF3243B17A3CCFA9E9441A" ma:contentTypeVersion="5" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="6b288f72ed777e9b1aae4ed183f5678c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7a2aa5ce-9268-4b11-b8eb-4b0ce9691849" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fb49ff9540079cd935bf7e769512398a" ns2:_="">
     <xsd:import namespace="7a2aa5ce-9268-4b11-b8eb-4b0ce9691849"/>
@@ -1319,6 +1310,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5A09CFD-DE79-4514-8D9E-8327453187AE}">
   <ds:schemaRefs>
@@ -1329,14 +1329,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F9B1BA4-1007-4EDD-9D02-AF3339A6D0CD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73027F6-8459-4821-9782-8EA37E764BC2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1352,4 +1344,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F9B1BA4-1007-4EDD-9D02-AF3339A6D0CD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>